<commit_message>
HTML description in Indicator aggregation.xlsx
</commit_message>
<xml_diff>
--- a/Indicator aggregation.xlsx
+++ b/Indicator aggregation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ljmac/Google Drive/PhD/R code/Compound Risk/Compound Risk/covid/compoundriskdata/Annotation and Data Architecture/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bennotkin/Documents/world-bank/crm/compoundriskdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BE3BDD-9C8F-AB4A-AC69-73C86F5C40E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F00B675-2171-7A44-95AB-6BC01051835E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3700" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="3" xr2:uid="{B42EF1BE-965E-B741-ADF0-C68AD4A5C459}"/>
+    <workbookView xWindow="100" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="3" xr2:uid="{B42EF1BE-965E-B741-ADF0-C68AD4A5C459}"/>
   </bookViews>
   <sheets>
     <sheet name="Emerging Risk" sheetId="1" r:id="rId1"/>
@@ -1218,9 +1218,6 @@
     <t>Oxford Lockdown rollback index (Oxford University - Blavatnik, source)</t>
   </si>
   <si>
-    <t>A measure of availability and access to food</t>
-  </si>
-  <si>
     <t>A measure of a country's exposure and resilience to a variety of natural and seasonal hazards, including earthquakes, tsunamis, floods, cyclones, storm surge, pests and drought risk</t>
   </si>
   <si>
@@ -1237,6 +1234,49 @@
   </si>
   <si>
     <t>A measure of of a country's response capacity to a pandemic (note: indicators for emerging risk are targetted specifically at COVID-related dynamic)</t>
+  </si>
+  <si>
+    <t>&lt;h3&gt;Food Security&lt;/h3&gt;
+Food insecurity within the CRM is defined as contexts where people do not have adequate physical, social or economic access to food. This holistic definition recognizes that there is no single metric of food insecurity, and rather demands multi-dimensional measures covering all aspects related to access to sufficient amounts of safe and nutritious food.
+&lt;h4&gt;Key resources&lt;/h4&gt;
+&lt;ul&gt;
+    &lt;li&gt;&lt;a href="https://www.worldbank.org/en/programs/famine-early-action-mechanism"&gt;Famine Action Mechanism (FAM)&lt;/a&gt;&lt;/li&gt;
+    &lt;li&gt;&lt;a href="https://fews.net"&gt;FEWS NET&lt;/a&gt;&lt;/li&gt;
+&lt;/ul&gt;
+&lt;h4&gt;Key contacts&lt;/h4&gt;
+&lt;ul&gt;
+    &lt;li&gt;&lt;a href="mailto:mgautam@worldbank.org"&gt;Madhur Gautam&lt;/a&gt;, &lt;i&gt;Lead Economist, Agriculture Global Practice&lt;/i&gt;&lt;/li&gt;
+    &lt;li&gt;&lt;a href="mailto:zcarmichael@worldbank.org"&gt;Zacharey Carmichael&lt;/a&gt;, &lt;i&gt;Team Leader for the Famine Action Mechanism&lt;/i&gt;&lt;/li&gt;
+&lt;/ul&gt;
+&lt;h4&gt;Underlying indicators&lt;/h4&gt;
+&lt;table&gt;
+	&lt;tr&gt;
+		&lt;td&gt;&lt;b&gt;Underlying Vulnerability&lt;/b&gt;&lt;/td&gt;
+	&lt;/tr&gt;
+	&lt;tr&gt;
+		&lt;td&gt;
+			&lt;a href="https://www.researchgate.net/publication/338972365_The_Proteus_composite_index_Towards_a_better_metric_for_global_food_security"&gt;Proteus Composite Index&lt;/a&gt;&lt;/td&gt;
+		&lt;!--&lt;td&gt;Index of multidimensional aspects of food security made up of grouped indicators for: Availability; Access; Utilization; and Stability&lt;/td&gt;--&gt;
+	&lt;/tr&gt;
+	&lt;tr&gt;
+		&lt;td&gt;&lt;b&gt;Emerging Threat&lt;/b&gt;&lt;/td&gt;
+	&lt;/tr&gt;
+	&lt;tr&gt;
+		&lt;td&gt;
+			&lt;a href="https://www.wfp.org/publications/fao-wfp-early-warning-analysis-acute-food-insecurity-hotspots-november-2020"&gt;FAO WFP Warning&lt;/a&gt;&lt;/td&gt;
+		&lt;!--&lt;td&gt;Food security early warning released jointly by FAO and WFP&lt;/td&gt;--&gt;
+	&lt;/tr&gt;
+	&lt;tr&gt;
+		&lt;td&gt;
+			&lt;a href="https://fews.net/"&gt;FEWSNET Score&lt;/a&gt;&lt;/td&gt;
+		&lt;!--&lt;td&gt;FEWSNET IPC classification (near term) adjusted&lt;/td&gt;--&gt;
+	&lt;/tr&gt;
+	&lt;tr&gt;
+		&lt;td&gt;
+			&lt;a href=""&gt;Food Price Volatility (Secondary Indicator)&lt;/a&gt;&lt;/td&gt;
+		&lt;!--&lt;td&gt;Food Price Inflation (gathered by WB’s Food Price Monitor)&lt;/td&gt;--&gt;
+	&lt;/tr&gt;
+&lt;/table&gt;</t>
   </si>
 </sst>
 </file>
@@ -1828,96 +1868,6 @@
     <xf numFmtId="0" fontId="3" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1982,6 +1932,96 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3024,13 +3064,13 @@
       </c>
     </row>
     <row r="2" spans="1:95" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="99" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="61"/>
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="101"/>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
@@ -3132,10 +3172,10 @@
       <c r="C3" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="D3" s="69" t="s">
+      <c r="D3" s="109" t="s">
         <v>135</v>
       </c>
-      <c r="E3" s="65" t="s">
+      <c r="E3" s="105" t="s">
         <v>136</v>
       </c>
       <c r="F3" s="14"/>
@@ -3239,8 +3279,8 @@
       <c r="C4" s="48" t="s">
         <v>118</v>
       </c>
-      <c r="D4" s="69"/>
-      <c r="E4" s="66"/>
+      <c r="D4" s="109"/>
+      <c r="E4" s="106"/>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
@@ -3342,8 +3382,8 @@
       <c r="C5" s="48" t="s">
         <v>119</v>
       </c>
-      <c r="D5" s="69"/>
-      <c r="E5" s="66"/>
+      <c r="D5" s="109"/>
+      <c r="E5" s="106"/>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
@@ -3445,8 +3485,8 @@
       <c r="C6" s="48" t="s">
         <v>120</v>
       </c>
-      <c r="D6" s="69"/>
-      <c r="E6" s="67"/>
+      <c r="D6" s="109"/>
+      <c r="E6" s="107"/>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
@@ -3538,13 +3578,13 @@
       <c r="CP6" s="14"/>
     </row>
     <row r="7" spans="1:95" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="99" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="61"/>
+      <c r="B7" s="100"/>
+      <c r="C7" s="100"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="101"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
@@ -3645,10 +3685,10 @@
       <c r="C8" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="70" t="s">
+      <c r="D8" s="110" t="s">
         <v>71</v>
       </c>
-      <c r="E8" s="77" t="s">
+      <c r="E8" s="94" t="s">
         <v>72</v>
       </c>
       <c r="F8" s="14"/>
@@ -3751,8 +3791,8 @@
       <c r="C9" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="71"/>
-      <c r="E9" s="78"/>
+      <c r="D9" s="111"/>
+      <c r="E9" s="95"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
@@ -3853,8 +3893,8 @@
       <c r="C10" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="71"/>
-      <c r="E10" s="78"/>
+      <c r="D10" s="111"/>
+      <c r="E10" s="95"/>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
@@ -3955,8 +3995,8 @@
       <c r="C11" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="D11" s="71"/>
-      <c r="E11" s="78"/>
+      <c r="D11" s="111"/>
+      <c r="E11" s="95"/>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
@@ -4057,8 +4097,8 @@
       <c r="C12" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="D12" s="71"/>
-      <c r="E12" s="78"/>
+      <c r="D12" s="111"/>
+      <c r="E12" s="95"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
@@ -4159,8 +4199,8 @@
       <c r="C13" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="72"/>
-      <c r="E13" s="79"/>
+      <c r="D13" s="112"/>
+      <c r="E13" s="96"/>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
@@ -4252,13 +4292,13 @@
       <c r="CP13" s="14"/>
     </row>
     <row r="14" spans="1:95" s="3" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="62" t="s">
+      <c r="A14" s="102" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="64"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
+      <c r="B14" s="104"/>
+      <c r="C14" s="104"/>
+      <c r="D14" s="104"/>
+      <c r="E14" s="104"/>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -4359,10 +4399,10 @@
       <c r="C15" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="69" t="s">
+      <c r="D15" s="109" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="68" t="s">
+      <c r="E15" s="108" t="s">
         <v>12</v>
       </c>
       <c r="F15" s="14"/>
@@ -4465,8 +4505,8 @@
       <c r="C16" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="69"/>
-      <c r="E16" s="68"/>
+      <c r="D16" s="109"/>
+      <c r="E16" s="108"/>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
@@ -4558,13 +4598,13 @@
       <c r="CP16" s="14"/>
     </row>
     <row r="17" spans="1:95" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="59" t="s">
+      <c r="A17" s="99" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="60"/>
-      <c r="C17" s="60"/>
-      <c r="D17" s="60"/>
-      <c r="E17" s="61"/>
+      <c r="B17" s="100"/>
+      <c r="C17" s="100"/>
+      <c r="D17" s="100"/>
+      <c r="E17" s="101"/>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
@@ -4666,10 +4706,10 @@
       <c r="C18" s="53" t="s">
         <v>129</v>
       </c>
-      <c r="D18" s="80" t="s">
+      <c r="D18" s="97" t="s">
         <v>130</v>
       </c>
-      <c r="E18" s="80" t="s">
+      <c r="E18" s="97" t="s">
         <v>13</v>
       </c>
       <c r="F18" s="14"/>
@@ -4773,8 +4813,8 @@
       <c r="C19" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="D19" s="81"/>
-      <c r="E19" s="80"/>
+      <c r="D19" s="98"/>
+      <c r="E19" s="97"/>
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -4876,8 +4916,8 @@
       <c r="C20" s="54" t="s">
         <v>125</v>
       </c>
-      <c r="D20" s="81"/>
-      <c r="E20" s="80"/>
+      <c r="D20" s="98"/>
+      <c r="E20" s="97"/>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
@@ -4979,8 +5019,8 @@
       <c r="C21" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="81"/>
-      <c r="E21" s="80"/>
+      <c r="D21" s="98"/>
+      <c r="E21" s="97"/>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
@@ -5073,13 +5113,13 @@
       <c r="CQ21" s="14"/>
     </row>
     <row r="22" spans="1:95" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="62" t="s">
+      <c r="A22" s="102" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="63"/>
-      <c r="C22" s="63"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="63"/>
+      <c r="B22" s="103"/>
+      <c r="C22" s="103"/>
+      <c r="D22" s="103"/>
+      <c r="E22" s="103"/>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
@@ -5181,10 +5221,10 @@
       <c r="C23" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="D23" s="88" t="s">
+      <c r="D23" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="E23" s="76" t="s">
+      <c r="E23" s="93" t="s">
         <v>15</v>
       </c>
       <c r="F23" s="14"/>
@@ -5288,8 +5328,8 @@
       <c r="C24" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="D24" s="88"/>
-      <c r="E24" s="76"/>
+      <c r="D24" s="89"/>
+      <c r="E24" s="93"/>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
@@ -5391,8 +5431,8 @@
       <c r="C25" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="D25" s="88"/>
-      <c r="E25" s="76"/>
+      <c r="D25" s="89"/>
+      <c r="E25" s="93"/>
       <c r="F25" s="14"/>
       <c r="G25" s="14" t="s">
         <v>75</v>
@@ -5496,8 +5536,8 @@
       <c r="C26" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="88"/>
-      <c r="E26" s="76"/>
+      <c r="D26" s="89"/>
+      <c r="E26" s="93"/>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
@@ -5599,8 +5639,8 @@
       <c r="C27" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="D27" s="88"/>
-      <c r="E27" s="76"/>
+      <c r="D27" s="89"/>
+      <c r="E27" s="93"/>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
@@ -5702,8 +5742,8 @@
       <c r="C28" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="D28" s="88"/>
-      <c r="E28" s="76"/>
+      <c r="D28" s="89"/>
+      <c r="E28" s="93"/>
       <c r="F28" s="14"/>
       <c r="G28" s="14"/>
       <c r="H28" s="14"/>
@@ -5805,8 +5845,8 @@
       <c r="C29" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="D29" s="88"/>
-      <c r="E29" s="76"/>
+      <c r="D29" s="89"/>
+      <c r="E29" s="93"/>
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
       <c r="H29" s="14"/>
@@ -5899,13 +5939,13 @@
       <c r="CQ29" s="14"/>
     </row>
     <row r="30" spans="1:95" s="5" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="73" t="s">
+      <c r="A30" s="90" t="s">
         <v>36</v>
       </c>
-      <c r="B30" s="74"/>
-      <c r="C30" s="74"/>
-      <c r="D30" s="74"/>
-      <c r="E30" s="75"/>
+      <c r="B30" s="91"/>
+      <c r="C30" s="91"/>
+      <c r="D30" s="91"/>
+      <c r="E30" s="92"/>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
@@ -6007,10 +6047,10 @@
       <c r="C31" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="D31" s="82" t="s">
+      <c r="D31" s="83" t="s">
         <v>73</v>
       </c>
-      <c r="E31" s="85" t="s">
+      <c r="E31" s="86" t="s">
         <v>74</v>
       </c>
       <c r="F31" s="14"/>
@@ -6114,8 +6154,8 @@
       <c r="C32" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="D32" s="83"/>
-      <c r="E32" s="86"/>
+      <c r="D32" s="84"/>
+      <c r="E32" s="87"/>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
       <c r="H32" s="14"/>
@@ -6217,8 +6257,8 @@
       <c r="C33" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="D33" s="84"/>
-      <c r="E33" s="87"/>
+      <c r="D33" s="85"/>
+      <c r="E33" s="88"/>
       <c r="F33" s="14"/>
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
@@ -6323,17 +6363,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="D31:D33"/>
-    <mergeCell ref="E31:E33"/>
-    <mergeCell ref="D23:D29"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="E23:E29"/>
-    <mergeCell ref="E8:E13"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="E18:E21"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A17:E17"/>
     <mergeCell ref="A22:E22"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="E3:E6"/>
@@ -6341,6 +6370,17 @@
     <mergeCell ref="D3:D6"/>
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="D8:D13"/>
+    <mergeCell ref="E8:E13"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="D31:D33"/>
+    <mergeCell ref="E31:E33"/>
+    <mergeCell ref="D23:D29"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="E23:E29"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -6372,7 +6412,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.5" style="109" customWidth="1"/>
+    <col min="1" max="1" width="41.5" style="79" customWidth="1"/>
     <col min="2" max="2" width="53" customWidth="1"/>
     <col min="3" max="3" width="24.5" customWidth="1"/>
     <col min="4" max="4" width="62.33203125" customWidth="1"/>
@@ -6380,7 +6420,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="73" t="s">
         <v>18</v>
       </c>
       <c r="B1" s="29" t="s">
@@ -6397,15 +6437,15 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="99" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
     </row>
     <row r="3" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="104" t="s">
+      <c r="A3" s="74" t="s">
         <v>84</v>
       </c>
       <c r="B3" s="39" t="s">
@@ -6422,34 +6462,34 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="99" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
+      <c r="B4" s="100"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
     </row>
     <row r="5" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="105" t="s">
+      <c r="A5" s="75" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="111" t="s">
+      <c r="B5" s="81" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="111"/>
-      <c r="D5" s="111"/>
-      <c r="E5" s="111"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
     </row>
     <row r="6" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="62" t="s">
+      <c r="A6" s="102" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="64"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
+      <c r="B6" s="104"/>
+      <c r="C6" s="104"/>
+      <c r="D6" s="104"/>
     </row>
     <row r="7" spans="1:7" ht="159" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="106" t="s">
+      <c r="A7" s="76" t="s">
         <v>85</v>
       </c>
       <c r="B7" s="9" t="s">
@@ -6469,12 +6509,12 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="99" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="60"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
+      <c r="B8" s="100"/>
+      <c r="C8" s="100"/>
+      <c r="D8" s="100"/>
       <c r="G8" s="46"/>
     </row>
     <row r="9" spans="1:7" ht="51" x14ac:dyDescent="0.2">
@@ -6498,16 +6538,16 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="62" t="s">
+      <c r="A10" s="102" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="64"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
+      <c r="B10" s="104"/>
+      <c r="C10" s="104"/>
+      <c r="D10" s="104"/>
       <c r="G10" s="47"/>
     </row>
     <row r="11" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A11" s="107" t="s">
+      <c r="A11" s="77" t="s">
         <v>82</v>
       </c>
       <c r="B11" s="40" t="s">
@@ -6516,35 +6556,35 @@
       <c r="C11" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="D11" s="100" t="s">
+      <c r="D11" s="70" t="s">
         <v>174</v>
       </c>
-      <c r="E11" s="101" t="s">
+      <c r="E11" s="71" t="s">
         <v>175</v>
       </c>
-      <c r="F11" s="102"/>
+      <c r="F11" s="72"/>
       <c r="G11" s="46"/>
     </row>
     <row r="12" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="73" t="s">
+      <c r="A12" s="90" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="74"/>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
+      <c r="B12" s="91"/>
+      <c r="C12" s="91"/>
+      <c r="D12" s="91"/>
       <c r="G12" s="45"/>
     </row>
     <row r="13" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="95" t="s">
+      <c r="A13" s="65" t="s">
         <v>171</v>
       </c>
-      <c r="B13" s="97" t="s">
+      <c r="B13" s="67" t="s">
         <v>172</v>
       </c>
-      <c r="C13" s="98" t="s">
+      <c r="C13" s="68" t="s">
         <v>97</v>
       </c>
-      <c r="D13" s="99" t="s">
+      <c r="D13" s="69" t="s">
         <v>173</v>
       </c>
       <c r="E13" s="35"/>
@@ -6553,15 +6593,15 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="73" t="s">
+      <c r="A14" s="90" t="s">
         <v>89</v>
       </c>
-      <c r="B14" s="74"/>
-      <c r="C14" s="74"/>
-      <c r="D14" s="74"/>
+      <c r="B14" s="91"/>
+      <c r="C14" s="91"/>
+      <c r="D14" s="91"/>
     </row>
     <row r="15" spans="1:7" ht="248" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="108" t="s">
+      <c r="A15" s="78" t="s">
         <v>87</v>
       </c>
       <c r="B15" s="41" t="s">
@@ -6677,7 +6717,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6687,19 +6727,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="59" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="89" t="s">
+      <c r="B1" s="59" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="34" x14ac:dyDescent="0.2">
@@ -6707,7 +6747,7 @@
         <v>70</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="51" x14ac:dyDescent="0.2">
@@ -6715,7 +6755,7 @@
         <v>46</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="34" x14ac:dyDescent="0.2">
@@ -6723,7 +6763,7 @@
         <v>35</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="51" x14ac:dyDescent="0.2">
@@ -6731,7 +6771,7 @@
         <v>45</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="53" customHeight="1" x14ac:dyDescent="0.2">
@@ -6739,7 +6779,7 @@
         <v>36</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="34" x14ac:dyDescent="0.2">
@@ -6747,11 +6787,11 @@
         <v>89</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B24" s="112" t="s">
+      <c r="B24" s="82" t="s">
         <v>83</v>
       </c>
     </row>
@@ -6784,16 +6824,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="59" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="89" t="s">
+      <c r="B1" s="59" t="s">
         <v>137</v>
       </c>
-      <c r="C1" s="89" t="s">
+      <c r="C1" s="59" t="s">
         <v>140</v>
       </c>
-      <c r="D1" s="89" t="s">
+      <c r="D1" s="59" t="s">
         <v>141</v>
       </c>
     </row>
@@ -6804,13 +6844,13 @@
       <c r="B2" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="90" t="s">
+      <c r="C2" s="60" t="s">
         <v>84</v>
       </c>
       <c r="D2" t="s">
         <v>143</v>
       </c>
-      <c r="E2" s="91"/>
+      <c r="E2" s="61"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -6819,7 +6859,7 @@
       <c r="B3" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="92" t="s">
+      <c r="C3" s="62" t="s">
         <v>88</v>
       </c>
       <c r="D3" t="s">
@@ -6833,7 +6873,7 @@
       <c r="B4" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="93" t="s">
+      <c r="C4" s="63" t="s">
         <v>85</v>
       </c>
       <c r="D4" t="s">
@@ -6847,7 +6887,7 @@
       <c r="B5" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="94" t="s">
+      <c r="C5" s="64" t="s">
         <v>86</v>
       </c>
       <c r="D5" t="s">
@@ -6861,7 +6901,7 @@
       <c r="B6" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="90" t="s">
+      <c r="C6" s="60" t="s">
         <v>82</v>
       </c>
       <c r="D6" t="s">
@@ -6875,7 +6915,7 @@
       <c r="B7" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="95" t="s">
+      <c r="C7" s="65" t="s">
         <v>171</v>
       </c>
       <c r="D7" t="s">
@@ -6889,7 +6929,7 @@
       <c r="B8" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="96" t="s">
+      <c r="C8" s="66" t="s">
         <v>87</v>
       </c>
       <c r="D8" t="s">
@@ -6906,7 +6946,7 @@
       <c r="C9" s="57" t="s">
         <v>115</v>
       </c>
-      <c r="D9" s="110" t="s">
+      <c r="D9" s="80" t="s">
         <v>177</v>
       </c>
     </row>
@@ -6920,7 +6960,7 @@
       <c r="C10" s="57" t="s">
         <v>114</v>
       </c>
-      <c r="D10" s="110" t="s">
+      <c r="D10" s="80" t="s">
         <v>176</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Re-added html to Indicator aggregation.xlsx
</commit_message>
<xml_diff>
--- a/Indicator aggregation.xlsx
+++ b/Indicator aggregation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bennotkin/Documents/world-bank/crm/compoundriskdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34463BDC-82CD-4A4A-8E89-1B1614D47138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FB9889-8AE1-434E-AF1C-07F56D3CF1C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7940" yWindow="22060" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7940" yWindow="22060" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Existing Risk" sheetId="2" r:id="rId1"/>
@@ -405,9 +405,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>A measure of availability and access to food</t>
-  </si>
-  <si>
     <t>A measure of institutional and social fragility as well as likehood of violent conflict</t>
   </si>
   <si>
@@ -1519,6 +1516,51 @@
   </si>
   <si>
     <t>Point change in the Economist Intelligence Unit’s Country-level Operational Risk Score: a multi-dimension index tracking macro-fiscal conditions updated on a monthly basis</t>
+  </si>
+  <si>
+    <t>&lt;h3&gt;Food Security&lt;/h3&gt;
+Food insecurity within the CRM is defined as contexts where people do not have adequate physical, social or economic access to food. This holistic definition recognizes that there is no single metric of food insecurity, and rather demands multi-dimensional measures covering all aspects related to access to sufficient amounts of safe and nutritious food.
+&lt;h4&gt;Key resources&lt;/h4&gt;
+&lt;ul&gt;
+    &lt;li&gt;&lt;a href="https://worldbankgroup.sharepoint.com/sites/agriculture/pages/home.aspx"&gt;Agriculture and Food Global Practice&lt;/a&gt;&lt;/li&gt;
+    &lt;li&gt;&lt;a href=""&gt;Agriculture Observatory&lt;/a&gt;&lt;/li&gt;
+    &lt;li&gt;&lt;a href="https://www.worldbank.org/en/programs/famine-early-action-mechanism"&gt;Famine Action Mechanism (FAM)&lt;/a&gt;&lt;/li&gt;
+    &lt;li&gt;&lt;a href="https://fews.net"&gt;FEWS NET&lt;/a&gt;&lt;/li&gt;
+&lt;/ul&gt;
+&lt;h4&gt;Key contacts&lt;/h4&gt;
+&lt;ul&gt;
+    &lt;li&gt;&lt;a href="mailto:mgautam@worldbank.org"&gt;Madhur Gautam&lt;/a&gt;, &lt;i&gt;Lead Economist, Agriculture Global Practice&lt;/i&gt;&lt;/li&gt;
+    &lt;li&gt;&lt;a href="mailto:zcarmichael@worldbank.org"&gt;Zacharey Carmichael&lt;/a&gt;, &lt;i&gt;Team Leader for the Famine Action Mechanism&lt;/i&gt;&lt;/li&gt;
+&lt;/ul&gt;
+&lt;h4&gt;Underlying indicators&lt;/h4&gt;
+&lt;table&gt;
+	&lt;tr&gt;
+		&lt;td&gt;&lt;b&gt;Underlying Vulnerability&lt;/b&gt;&lt;/td&gt;
+	&lt;/tr&gt;
+	&lt;tr&gt;
+		&lt;td&gt;
+			&lt;a href="https://www.researchgate.net/publication/338972365_The_Proteus_composite_index_Towards_a_better_metric_for_global_food_security"&gt;Proteus Composite Index&lt;/a&gt;&lt;/td&gt;
+		&lt;!--&lt;td&gt;Index of multidimensional aspects of food security made up of grouped indicators for: Availability; Access; Utilization; and Stability&lt;/td&gt;--&gt;
+	&lt;/tr&gt;
+	&lt;tr&gt;
+		&lt;td&gt;&lt;b&gt;Emerging Threat&lt;/b&gt;&lt;/td&gt;
+	&lt;/tr&gt;
+	&lt;tr&gt;
+		&lt;td&gt;
+			&lt;a href="https://www.wfp.org/publications/fao-wfp-early-warning-analysis-acute-food-insecurity-hotspots-november-2020"&gt;FAO WFP Warning&lt;/a&gt;&lt;/td&gt;
+		&lt;!--&lt;td&gt;Food security early warning released jointly by FAO and WFP&lt;/td&gt;--&gt;
+	&lt;/tr&gt;
+	&lt;tr&gt;
+		&lt;td&gt;
+			&lt;a href="https://fews.net/"&gt;FEWSNET Score&lt;/a&gt;&lt;/td&gt;
+		&lt;!--&lt;td&gt;FEWSNET IPC classification (near term) adjusted&lt;/td&gt;--&gt;
+	&lt;/tr&gt;
+	&lt;tr&gt;
+		&lt;td&gt;
+			&lt;a href=""&gt;Food Price Volatility (Secondary Indicator)&lt;/a&gt;&lt;/td&gt;
+		&lt;!--&lt;td&gt;Food Price Inflation (gathered by WB’s Food Price Monitor)&lt;/td&gt;--&gt;
+	&lt;/tr&gt;
+&lt;/table&gt;</t>
   </si>
 </sst>
 </file>
@@ -3404,7 +3446,7 @@
         <v>57</v>
       </c>
       <c r="E3" s="98" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3423,17 +3465,17 @@
     </row>
     <row r="5" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="52" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B5" s="53" t="s">
         <v>58</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D5" s="55"/>
       <c r="E5" s="97" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="56"/>
@@ -3457,17 +3499,17 @@
     </row>
     <row r="7" spans="1:12" ht="88" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="58" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="60" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" s="59" t="s">
         <v>114</v>
-      </c>
-      <c r="B7" s="60" t="s">
-        <v>113</v>
-      </c>
-      <c r="C7" s="59" t="s">
-        <v>115</v>
       </c>
       <c r="D7" s="61"/>
       <c r="E7" s="96" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G7" s="62"/>
       <c r="H7" s="124"/>
@@ -3547,13 +3589,13 @@
         <v>68</v>
       </c>
       <c r="C12" s="77" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D12" s="78" t="s">
         <v>69</v>
       </c>
       <c r="E12" s="95" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G12" s="62" t="s">
         <v>59</v>
@@ -3576,7 +3618,7 @@
         <v>71</v>
       </c>
       <c r="C14" s="81" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D14" s="82" t="s">
         <v>72</v>
@@ -3749,7 +3791,7 @@
     </row>
     <row r="3" spans="1:94" s="9" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>5</v>
@@ -3758,7 +3800,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="136" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -3955,7 +3997,7 @@
     </row>
     <row r="5" spans="1:94" s="9" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>10</v>
@@ -4154,7 +4196,7 @@
     </row>
     <row r="7" spans="1:94" s="18" customFormat="1" ht="103" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B7" s="20" t="s">
         <v>13</v>
@@ -4163,7 +4205,7 @@
         <v>14</v>
       </c>
       <c r="D7" s="133" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -4257,7 +4299,7 @@
     </row>
     <row r="8" spans="1:94" s="18" customFormat="1" ht="119" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B8" s="22" t="s">
         <v>15</v>
@@ -4747,16 +4789,16 @@
     </row>
     <row r="13" spans="1:94" s="24" customFormat="1" ht="69" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>216</v>
+      </c>
+      <c r="C13" s="99" t="s">
         <v>125</v>
       </c>
-      <c r="B13" s="26" t="s">
-        <v>217</v>
-      </c>
-      <c r="C13" s="99" t="s">
+      <c r="D13" s="100" t="s">
         <v>126</v>
-      </c>
-      <c r="D13" s="100" t="s">
-        <v>127</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -4949,16 +4991,16 @@
     </row>
     <row r="15" spans="1:94" s="24" customFormat="1" ht="128" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B15" s="28" t="s">
         <v>22</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D15" s="139" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -5053,13 +5095,13 @@
     </row>
     <row r="16" spans="1:94" s="24" customFormat="1" ht="119" x14ac:dyDescent="0.2">
       <c r="A16" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="B16" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="C16" s="29" t="s">
         <v>131</v>
-      </c>
-      <c r="C16" s="29" t="s">
-        <v>132</v>
       </c>
       <c r="D16" s="140"/>
       <c r="E16" s="4"/>
@@ -5257,7 +5299,7 @@
     </row>
     <row r="18" spans="1:94" s="24" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A18" s="101" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B18" s="28" t="s">
         <v>26</v>
@@ -5359,13 +5401,13 @@
     </row>
     <row r="19" spans="1:94" s="24" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A19" s="101" t="s">
+        <v>132</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="C19" s="29" t="s">
         <v>133</v>
-      </c>
-      <c r="B19" s="28" t="s">
-        <v>216</v>
-      </c>
-      <c r="C19" s="29" t="s">
-        <v>134</v>
       </c>
       <c r="D19" s="141"/>
       <c r="E19" s="4"/>
@@ -5565,7 +5607,7 @@
         <v>31</v>
       </c>
       <c r="C21" s="32" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D21" s="142" t="s">
         <v>29</v>
@@ -5669,7 +5711,7 @@
         <v>33</v>
       </c>
       <c r="C22" s="32" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D22" s="143"/>
       <c r="E22" s="4"/>
@@ -5773,7 +5815,7 @@
         <v>36</v>
       </c>
       <c r="C23" s="32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D23" s="143"/>
       <c r="E23" s="4"/>
@@ -5875,7 +5917,7 @@
         <v>38</v>
       </c>
       <c r="C24" s="32" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D24" s="143"/>
       <c r="E24" s="4"/>
@@ -5971,13 +6013,13 @@
     </row>
     <row r="25" spans="1:94" s="24" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="30" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B25" s="31" t="s">
         <v>39</v>
       </c>
       <c r="C25" s="32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D25" s="143"/>
       <c r="E25" s="4"/>
@@ -6175,13 +6217,13 @@
     </row>
     <row r="27" spans="1:94" s="24" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B27" s="31" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C27" s="32" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D27" s="143"/>
       <c r="E27" s="4"/>
@@ -6477,16 +6519,16 @@
     </row>
     <row r="30" spans="1:94" s="33" customFormat="1" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B30" s="35" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C30" s="93" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D30" s="130" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -6581,10 +6623,10 @@
     </row>
     <row r="31" spans="1:94" s="33" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="34" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B31" s="35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C31" s="93"/>
       <c r="D31" s="131"/>
@@ -6681,13 +6723,13 @@
     </row>
     <row r="32" spans="1:94" s="33" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="B32" s="35" t="s">
+        <v>149</v>
+      </c>
+      <c r="C32" s="93" t="s">
         <v>142</v>
-      </c>
-      <c r="B32" s="35" t="s">
-        <v>150</v>
-      </c>
-      <c r="C32" s="93" t="s">
-        <v>143</v>
       </c>
       <c r="D32" s="131"/>
       <c r="E32" s="4"/>
@@ -6940,7 +6982,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>74</v>
@@ -6954,7 +6996,7 @@
     </row>
     <row r="2" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="125" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B2" s="145"/>
       <c r="C2" s="145"/>
@@ -6962,77 +7004,77 @@
     </row>
     <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="87" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C4" s="87" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D4" s="94" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="87" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C5" s="87" t="s">
+        <v>198</v>
+      </c>
+      <c r="D5" s="120" t="s">
         <v>199</v>
-      </c>
-      <c r="D5" s="120" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="87" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C6" s="87" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D6" s="94" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="87" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C7" s="87" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D7" s="94" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A8" s="87" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C8" s="87" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D8" s="94" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="125" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B9" s="145"/>
       <c r="C9" s="145"/>
@@ -7040,10 +7082,10 @@
     </row>
     <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="87" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B10" s="86" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C10" s="87" t="s">
         <v>77</v>
@@ -7054,10 +7096,10 @@
     </row>
     <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="87" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C11" s="87" t="s">
         <v>77</v>
@@ -7068,86 +7110,86 @@
     </row>
     <row r="12" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="87" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C12" s="87" t="s">
         <v>79</v>
       </c>
       <c r="D12" s="94" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="87" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C13" s="87" t="s">
+        <v>183</v>
+      </c>
+      <c r="D13" s="94" t="s">
         <v>184</v>
-      </c>
-      <c r="D13" s="94" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="87" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C14" s="87" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D14" s="94" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="87" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C15" s="87" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D15" s="94" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="87" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C16" s="87" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D16" s="94" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A17" s="87" t="s">
+        <v>193</v>
+      </c>
+      <c r="B17" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="C17" s="87" t="s">
         <v>195</v>
       </c>
-      <c r="C17" s="87" t="s">
-        <v>196</v>
-      </c>
       <c r="D17" s="121" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -7188,8 +7230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7207,12 +7249,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="89" t="s">
-        <v>82</v>
+        <v>217</v>
       </c>
       <c r="E2" s="124"/>
       <c r="F2" s="124"/>
@@ -7225,7 +7267,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="89" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E3" s="124"/>
       <c r="F3" s="124"/>
@@ -7238,7 +7280,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="89" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E4" s="126"/>
       <c r="F4" s="126"/>
@@ -7248,10 +7290,10 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="89" t="s">
         <v>85</v>
-      </c>
-      <c r="B5" s="89" t="s">
-        <v>86</v>
       </c>
       <c r="E5" s="124"/>
       <c r="F5" s="124"/>
@@ -7264,7 +7306,7 @@
         <v>28</v>
       </c>
       <c r="B6" s="89" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E6" s="126"/>
       <c r="F6" s="126"/>
@@ -7277,7 +7319,7 @@
         <v>46</v>
       </c>
       <c r="B7" s="89" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E7" s="126"/>
       <c r="F7" s="126"/>
@@ -7287,10 +7329,10 @@
     </row>
     <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="89" t="s">
         <v>89</v>
-      </c>
-      <c r="B8" s="89" t="s">
-        <v>90</v>
       </c>
       <c r="E8" s="128"/>
       <c r="F8" s="128"/>
@@ -7327,7 +7369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="99" workbookViewId="0">
+    <sheetView zoomScaleNormal="99" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -7344,23 +7386,23 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="102" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B1" s="102" t="s">
         <v>80</v>
       </c>
       <c r="C1" s="102" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="102" t="s">
         <v>92</v>
-      </c>
-      <c r="D1" s="102" t="s">
-        <v>93</v>
       </c>
       <c r="E1" s="103"/>
       <c r="F1" s="104"/>
     </row>
     <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="104" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B2" s="104" t="s">
         <v>4</v>
@@ -7369,46 +7411,46 @@
         <v>54</v>
       </c>
       <c r="D2" s="104" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E2" s="106"/>
       <c r="F2" s="104"/>
     </row>
     <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="104" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" s="104" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="107" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D3" s="108" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E3" s="106"/>
       <c r="F3" s="104"/>
     </row>
     <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="104" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4" s="104" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C4" s="109" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D4" s="104" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E4" s="106"/>
       <c r="F4" s="104"/>
     </row>
     <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="104" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" s="104" t="s">
         <v>28</v>
@@ -7417,14 +7459,14 @@
         <v>60</v>
       </c>
       <c r="D5" s="108" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E5" s="106"/>
       <c r="F5" s="104"/>
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="104" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B6" s="104" t="s">
         <v>28</v>
@@ -7433,14 +7475,14 @@
         <v>63</v>
       </c>
       <c r="D6" s="104" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E6" s="106"/>
       <c r="F6" s="104"/>
     </row>
     <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="104" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B7" s="104" t="s">
         <v>46</v>
@@ -7449,62 +7491,62 @@
         <v>67</v>
       </c>
       <c r="D7" s="104" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E7" s="106"/>
       <c r="F7" s="104"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="104" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B8" s="104" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C8" s="111" t="s">
         <v>70</v>
       </c>
       <c r="D8" s="104" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E8" s="106"/>
       <c r="F8" s="104"/>
     </row>
     <row r="9" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="104" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B9" s="104" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="112" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" s="113" t="s">
         <v>101</v>
-      </c>
-      <c r="D9" s="113" t="s">
-        <v>102</v>
       </c>
       <c r="E9" s="106"/>
       <c r="F9" s="104"/>
     </row>
     <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="104" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B10" s="104" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="114" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D10" s="104" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E10" s="106"/>
       <c r="F10" s="104"/>
     </row>
     <row r="11" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="104" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B11" s="104" t="s">
         <v>4</v>
@@ -7513,30 +7555,30 @@
         <v>7</v>
       </c>
       <c r="D11" s="104" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E11" s="106"/>
       <c r="F11" s="104"/>
     </row>
     <row r="12" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="104" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B12" s="104" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="119" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" s="104" t="s">
         <v>103</v>
-      </c>
-      <c r="D12" s="104" t="s">
-        <v>104</v>
       </c>
       <c r="E12" s="106"/>
       <c r="F12" s="104"/>
     </row>
     <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="104" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B13" s="104" t="s">
         <v>12</v>
@@ -7545,126 +7587,126 @@
         <v>17</v>
       </c>
       <c r="D13" s="104" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E13" s="106"/>
       <c r="F13" s="104"/>
     </row>
     <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="104" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B14" s="104" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="119" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D14" s="104" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E14" s="106"/>
       <c r="F14" s="104"/>
     </row>
     <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="104" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B15" s="104" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C15" s="115" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D15" s="104" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E15" s="106"/>
       <c r="F15" s="104"/>
     </row>
     <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="104" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B16" s="104" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C16" s="116" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D16" s="104" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E16" s="106"/>
       <c r="F16" s="104"/>
     </row>
     <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="104" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B17" s="104" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C17" s="116" t="s">
         <v>23</v>
       </c>
       <c r="D17" s="104" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E17" s="106"/>
       <c r="F17" s="104"/>
     </row>
     <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="104" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B18" s="104" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C18" s="116" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D18" s="108" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E18" s="106"/>
       <c r="F18" s="104"/>
     </row>
     <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="104" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B19" s="104" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C19" s="116" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D19" s="108" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E19" s="106"/>
       <c r="F19" s="104"/>
     </row>
     <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="104" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B20" s="104" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C20" s="116" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D20" s="108" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E20" s="106"/>
       <c r="F20" s="104"/>
     </row>
     <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="104" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B21" s="104" t="s">
         <v>28</v>
@@ -7673,14 +7715,14 @@
         <v>30</v>
       </c>
       <c r="D21" s="104" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E21" s="106"/>
       <c r="F21" s="104"/>
     </row>
     <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="104" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B22" s="104" t="s">
         <v>28</v>
@@ -7689,46 +7731,46 @@
         <v>32</v>
       </c>
       <c r="D22" s="104" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E22" s="106"/>
       <c r="F22" s="104"/>
     </row>
     <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="104" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B23" s="104" t="s">
         <v>28</v>
       </c>
       <c r="C23" s="117" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D23" s="104" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E23" s="106"/>
       <c r="F23" s="104"/>
     </row>
     <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="104" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B24" s="104" t="s">
         <v>28</v>
       </c>
       <c r="C24" s="117" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D24" s="104" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E24" s="106"/>
       <c r="F24" s="104"/>
     </row>
     <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="104" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B25" s="104" t="s">
         <v>28</v>
@@ -7737,13 +7779,13 @@
         <v>35</v>
       </c>
       <c r="D25" s="104" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E25" s="106"/>
     </row>
     <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="104" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B26" s="104" t="s">
         <v>28</v>
@@ -7752,13 +7794,13 @@
         <v>37</v>
       </c>
       <c r="D26" s="104" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E26" s="106"/>
     </row>
     <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="104" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B27" s="104" t="s">
         <v>28</v>
@@ -7767,13 +7809,13 @@
         <v>43</v>
       </c>
       <c r="D27" s="104" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E27" s="106"/>
     </row>
     <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="104" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B28" s="104" t="s">
         <v>28</v>
@@ -7782,13 +7824,13 @@
         <v>40</v>
       </c>
       <c r="D28" s="104" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E28" s="106"/>
     </row>
     <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="104" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B29" s="104" t="s">
         <v>46</v>
@@ -7803,47 +7845,47 @@
     </row>
     <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="104" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B30" s="104" t="s">
         <v>46</v>
       </c>
       <c r="C30" s="118" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D30" s="104" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E30" s="106"/>
     </row>
     <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="104" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B31" s="104" t="s">
         <v>46</v>
       </c>
       <c r="C31" s="118" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D31" s="104" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E31" s="106"/>
       <c r="F31" s="104"/>
     </row>
     <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="104" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B32" s="104" t="s">
         <v>46</v>
       </c>
       <c r="C32" s="118" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E32" s="91"/>
     </row>

</xml_diff>